<commit_message>
add tables with Simpson Diversity. Update SI
</commit_message>
<xml_diff>
--- a/MainAnalysis/manuscript_tables.xlsx
+++ b/MainAnalysis/manuscript_tables.xlsx
@@ -11,9 +11,11 @@
     <sheet name="cntrl_even_res" sheetId="2" r:id="rId2"/>
     <sheet name="cntrl_rich_res" sheetId="3" r:id="rId3"/>
     <sheet name="cntrl_invsim_res" sheetId="4" r:id="rId4"/>
-    <sheet name="ancova_even" sheetId="5" r:id="rId5"/>
-    <sheet name="ancova_invsim" sheetId="6" r:id="rId6"/>
-    <sheet name="ancova_rich" sheetId="7" r:id="rId7"/>
+    <sheet name="cntrl_sim_res" sheetId="5" r:id="rId5"/>
+    <sheet name="ancova_even" sheetId="6" r:id="rId6"/>
+    <sheet name="ancova_invsim" sheetId="7" r:id="rId7"/>
+    <sheet name="ancova_sim" sheetId="8" r:id="rId8"/>
+    <sheet name="ancova_rich" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1000,7 +1002,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1009,243 +1011,153 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Term</t>
+          <t>term</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>DF</t>
+          <t>b</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>meansq</t>
+          <t>t-statistic</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>F-value</t>
+          <t>p_value</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>p.value</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>P</t>
+          <t>p-value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EvenScaled</t>
+          <t>(Intercept)</t>
         </is>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.36</v>
       </c>
       <c r="C2">
-        <v>0.448</v>
+        <v>0.202</v>
       </c>
       <c r="D2">
-        <v>0.448</v>
+        <v>1.786</v>
       </c>
       <c r="E2">
-        <v>0.673</v>
-      </c>
-      <c r="F2">
-        <v>0.413</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0.413</t>
+        <v>0.082</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.082</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TRT</t>
+          <t>SimScaled</t>
         </is>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.04</v>
       </c>
       <c r="C3">
-        <v>0.454</v>
+        <v>0.127</v>
       </c>
       <c r="D3">
-        <v>0.454</v>
+        <v>0.314</v>
       </c>
       <c r="E3">
-        <v>0.6820000000000001</v>
-      </c>
-      <c r="F3">
-        <v>0.41</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0.41</t>
+        <v>0.755</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.755</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Block</t>
+          <t>PC2</t>
         </is>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>-0.035</v>
       </c>
       <c r="C4">
-        <v>7.154</v>
+        <v>0.077</v>
       </c>
       <c r="D4">
-        <v>7.154</v>
+        <v>-0.46</v>
       </c>
       <c r="E4">
-        <v>10.746</v>
-      </c>
-      <c r="F4">
-        <v>0.001</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0.001**</t>
+        <v>0.648</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.648</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PC2</t>
+          <t>Block</t>
         </is>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.196</v>
       </c>
       <c r="C5">
-        <v>1.451</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D5">
-        <v>1.451</v>
+        <v>2.791</v>
       </c>
       <c r="E5">
-        <v>2.179</v>
-      </c>
-      <c r="F5">
-        <v>0.142</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>0.142</t>
+        <v>0.008</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.008**</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EvenScaled:TRT</t>
+          <t>SimScaled:PC2</t>
         </is>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.038</v>
       </c>
       <c r="C6">
-        <v>0.536</v>
+        <v>0.093</v>
       </c>
       <c r="D6">
-        <v>0.536</v>
+        <v>0.413</v>
       </c>
       <c r="E6">
-        <v>0.8050000000000001</v>
-      </c>
-      <c r="F6">
-        <v>0.371</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>0.371</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>EvenScaled:Block</t>
-        </is>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0.002</v>
-      </c>
-      <c r="D7">
-        <v>0.002</v>
-      </c>
-      <c r="E7">
-        <v>0.004</v>
-      </c>
-      <c r="F7">
-        <v>0.952</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>0.952</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>EvenScaled:PC2</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1.66</v>
-      </c>
-      <c r="D8">
-        <v>1.66</v>
-      </c>
-      <c r="E8">
-        <v>2.493</v>
-      </c>
-      <c r="F8">
-        <v>0.116</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>0.116</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Residuals</t>
-        </is>
-      </c>
-      <c r="B9">
-        <v>150</v>
-      </c>
-      <c r="C9">
-        <v>99.869</v>
-      </c>
-      <c r="D9">
-        <v>0.666</v>
+        <v>0.6820000000000001</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.682</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1301,27 +1213,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>InvSimScaled</t>
+          <t>EvenScaled</t>
         </is>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.99</v>
+        <v>0.448</v>
       </c>
       <c r="D2">
-        <v>0.99</v>
+        <v>0.448</v>
       </c>
       <c r="E2">
-        <v>1.504</v>
+        <v>0.673</v>
       </c>
       <c r="F2">
-        <v>0.222</v>
+        <v>0.413</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.222</t>
+          <t>0.413</t>
         </is>
       </c>
     </row>
@@ -1335,20 +1247,20 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.277</v>
+        <v>0.454</v>
       </c>
       <c r="D3">
-        <v>0.277</v>
+        <v>0.454</v>
       </c>
       <c r="E3">
-        <v>0.421</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="F3">
-        <v>0.517</v>
+        <v>0.41</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.517</t>
+          <t>0.41</t>
         </is>
       </c>
     </row>
@@ -1362,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>7.347</v>
+        <v>7.154</v>
       </c>
       <c r="D4">
-        <v>7.347</v>
+        <v>7.154</v>
       </c>
       <c r="E4">
-        <v>11.156</v>
+        <v>10.746</v>
       </c>
       <c r="F4">
         <v>0.001</v>
@@ -1389,101 +1301,101 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1.338</v>
+        <v>1.451</v>
       </c>
       <c r="D5">
-        <v>1.338</v>
+        <v>1.451</v>
       </c>
       <c r="E5">
-        <v>2.032</v>
+        <v>2.179</v>
       </c>
       <c r="F5">
-        <v>0.156</v>
+        <v>0.142</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.156</t>
+          <t>0.142</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>InvSimScaled:TRT</t>
+          <t>EvenScaled:TRT</t>
         </is>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.536</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.536</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.8050000000000001</v>
       </c>
       <c r="F6">
-        <v>0.988</v>
+        <v>0.371</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.988</t>
+          <t>0.371</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>InvSimScaled:Block</t>
+          <t>EvenScaled:Block</t>
         </is>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2.603</v>
+        <v>0.002</v>
       </c>
       <c r="D7">
-        <v>2.603</v>
+        <v>0.002</v>
       </c>
       <c r="E7">
-        <v>3.953</v>
+        <v>0.004</v>
       </c>
       <c r="F7">
-        <v>0.049</v>
+        <v>0.952</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.049*</t>
+          <t>0.952</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>InvSimScaled:PC2</t>
+          <t>EvenScaled:PC2</t>
         </is>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.24</v>
+        <v>1.66</v>
       </c>
       <c r="D8">
-        <v>0.24</v>
+        <v>1.66</v>
       </c>
       <c r="E8">
-        <v>0.364</v>
+        <v>2.493</v>
       </c>
       <c r="F8">
-        <v>0.547</v>
+        <v>0.116</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.547</t>
+          <t>0.116</t>
         </is>
       </c>
     </row>
@@ -1497,10 +1409,10 @@
         <v>150</v>
       </c>
       <c r="C9">
-        <v>98.779</v>
+        <v>99.869</v>
       </c>
       <c r="D9">
-        <v>0.659</v>
+        <v>0.666</v>
       </c>
     </row>
   </sheetData>
@@ -1556,6 +1468,516 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>InvSimScaled</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.99</v>
+      </c>
+      <c r="D2">
+        <v>0.99</v>
+      </c>
+      <c r="E2">
+        <v>1.504</v>
+      </c>
+      <c r="F2">
+        <v>0.222</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.222</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TRT</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.277</v>
+      </c>
+      <c r="D3">
+        <v>0.277</v>
+      </c>
+      <c r="E3">
+        <v>0.421</v>
+      </c>
+      <c r="F3">
+        <v>0.517</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.517</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Block</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>7.347</v>
+      </c>
+      <c r="D4">
+        <v>7.347</v>
+      </c>
+      <c r="E4">
+        <v>11.156</v>
+      </c>
+      <c r="F4">
+        <v>0.001</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.001**</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PC2</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.338</v>
+      </c>
+      <c r="D5">
+        <v>1.338</v>
+      </c>
+      <c r="E5">
+        <v>2.032</v>
+      </c>
+      <c r="F5">
+        <v>0.156</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.156</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>InvSimScaled:TRT</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.988</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.988</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>InvSimScaled:Block</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2.603</v>
+      </c>
+      <c r="D7">
+        <v>2.603</v>
+      </c>
+      <c r="E7">
+        <v>3.953</v>
+      </c>
+      <c r="F7">
+        <v>0.049</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.049*</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>InvSimScaled:PC2</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.24</v>
+      </c>
+      <c r="D8">
+        <v>0.24</v>
+      </c>
+      <c r="E8">
+        <v>0.364</v>
+      </c>
+      <c r="F8">
+        <v>0.547</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.547</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Residuals</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>150</v>
+      </c>
+      <c r="C9">
+        <v>98.779</v>
+      </c>
+      <c r="D9">
+        <v>0.659</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>meansq</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>F-value</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>p.value</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SimScaled</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.476</v>
+      </c>
+      <c r="D2">
+        <v>0.476</v>
+      </c>
+      <c r="E2">
+        <v>0.717</v>
+      </c>
+      <c r="F2">
+        <v>0.399</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.399</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TRT</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.357</v>
+      </c>
+      <c r="D3">
+        <v>0.357</v>
+      </c>
+      <c r="E3">
+        <v>0.537</v>
+      </c>
+      <c r="F3">
+        <v>0.465</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.465</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Block</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>7.452</v>
+      </c>
+      <c r="D4">
+        <v>7.452</v>
+      </c>
+      <c r="E4">
+        <v>11.211</v>
+      </c>
+      <c r="F4">
+        <v>0.001</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.001**</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PC2</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.398</v>
+      </c>
+      <c r="D5">
+        <v>1.398</v>
+      </c>
+      <c r="E5">
+        <v>2.103</v>
+      </c>
+      <c r="F5">
+        <v>0.149</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.149</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SimScaled:TRT</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.985</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.985</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SimScaled:Block</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2.005</v>
+      </c>
+      <c r="D7">
+        <v>2.005</v>
+      </c>
+      <c r="E7">
+        <v>3.016</v>
+      </c>
+      <c r="F7">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.084</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SimScaled:PC2</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.18</v>
+      </c>
+      <c r="D8">
+        <v>0.18</v>
+      </c>
+      <c r="E8">
+        <v>0.271</v>
+      </c>
+      <c r="F8">
+        <v>0.604</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.604</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Residuals</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>150</v>
+      </c>
+      <c r="C9">
+        <v>99.706</v>
+      </c>
+      <c r="D9">
+        <v>0.665</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Term</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>SS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>meansq</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>F-value</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>p.value</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>richScaled</t>
         </is>
       </c>

</xml_diff>